<commit_message>
update: mark posted movies as 완료
</commit_message>
<xml_diff>
--- a/movies_discover.xlsx
+++ b/movies_discover.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Movies" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Movies" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -8391,6 +8391,11 @@
       <c r="E291" t="n">
         <v>9948</v>
       </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>완</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">

</xml_diff>

<commit_message>
update: mark posted movies as 完了
</commit_message>
<xml_diff>
--- a/movies_discover.xlsx
+++ b/movies_discover.xlsx
@@ -6506,6 +6506,11 @@
           <t>완</t>
         </is>
       </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>완</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">

</xml_diff>